<commit_message>
- seperate <DialogData> struct file to DialogueInteraction.cs - tutorial system (구조만 설계해놓은 상태) 1. 튜토리얼 scene에 입장하면 튜토리얼 대화 송출 2. 튜토리얼 대화 엑셀 갱신
</commit_message>
<xml_diff>
--- a/Assets/Scripts/System/Interaction/Dialog/DialogueDB.xlsx
+++ b/Assets/Scripts/System/Interaction/Dialog/DialogueDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szun8/Documents/Develop/dragon-and-test/Assets/Scripts/System/Interaction/Dialog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c\Desktop\sieun\Develop\dragon-and-test\Assets\Scripts\System\Interaction\Dialog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6037CB8-75A3-3345-8128-AD381667B49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AF7869-9410-4F0F-A62D-47D35609C104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1480" windowWidth="27740" windowHeight="12840" xr2:uid="{62D67DF9-C02E-4B4B-9D5F-1B428BA22005}"/>
+    <workbookView xWindow="1065" yWindow="780" windowWidth="27735" windowHeight="12840" xr2:uid="{62D67DF9-C02E-4B4B-9D5F-1B428BA22005}"/>
   </bookViews>
   <sheets>
     <sheet name="DialogueEntity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="71">
   <si>
     <t>eventOrder</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -238,6 +238,102 @@
   </si>
   <si>
     <t>응? 돈이 부족한거 같아…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>허수아비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반가워! 오늘도 연습하러 왔네?
+다시 처음부터 연습해볼까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>먼저 움직이는 방법이야.
+WASD 키로 움직일 수 있어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격은 마우스 왼클릭, 구르기는 마우스 우클릭이야.
+나를 한 번 공격해볼래?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC나 오브젝트와 상호작용을 하고 싶다면 F키를 눌러봐</t>
+  </si>
+  <si>
+    <t>잘했어!! 기본적인 조작은 모두 마스터했어.
+이제 화투에 대해 알려줄게!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화투는 용들이 아주 오래전부터 즐긴 전통놀이이자, 가장 좋아하는 놀이 중 하나야!!</t>
+  </si>
+  <si>
+    <t>용들은 화투 놀이를 즐기기도 했지만,
+마법의 모포를 이용해 화투에 힘을 담아 전투에 사용하기도 했어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 화투 능력에 대해 자세히 알려주도록 할게!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하지만 이제는 화투 능력을 쓰는 용들이 거의 없는데…
+너는 아직도 쓰는구나??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화투의 힘을 이용한 능력은 굉장했지..
+동물왕국을 모두 저지했을 정도였으니까!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(뒤적뒤적..) 여기있다!
+이건 바로 화투 놀이중 하나인 섰다 족보책이야!
+이걸 받도록 해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>섰다 족보책을 한 번 펼쳐볼래??
+K키를 누르면 책을 볼 수 있어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>족보는 크게 광땡, 땡, 중간, 끗 순서대로야.
+각 카테고리를 살펴보면 어떤 화투패 조합이 있는지 알 수 있어.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금은 족보의 순서만 나와있지만 마법의 모포와 상호작용해서
+스킬을 얻으면 스킬 효과와 족보 시너지 효과를 알 수 있어!
+다양한 스킬을 얻고 사 용해보길 추천할께</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임시로 한 가지 스킬만 알려주도록 할까? 이건 화투패 능력 중 하나야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q키를 누르면 스킬을 사용할 수 있으니 한 번 사용해볼래?</t>
+  </si>
+  <si>
+    <t>잘했어!!
+이제 모든 훈련이 끝났으니 훈련장에서 나가봐도 좋아.
+이번엔 용과 시험에 꼭 통과하길 바라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>튜토리얼1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>튜토리얼2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>튜토리얼3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -245,7 +341,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -646,21 +742,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2825EA14-B14C-3842-BF84-4D0E376FD83F}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="122.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -680,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -697,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="38">
+    <row r="3" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -714,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -731,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -748,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="38">
+    <row r="6" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -765,7 +861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -782,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="38">
+    <row r="8" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -799,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="38">
+    <row r="9" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -816,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57">
+    <row r="10" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -833,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -853,7 +949,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -870,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -887,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -904,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -921,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -938,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -958,7 +1054,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -975,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -992,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1009,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="38">
+    <row r="21" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>6</v>
       </c>
@@ -1026,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="38">
+    <row r="22" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1043,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="38">
+    <row r="23" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1060,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1077,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="38">
+    <row r="25" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1097,7 +1193,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="19">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1114,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="19">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1131,7 +1227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="19">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1145,6 +1241,295 @@
         <v>49</v>
       </c>
       <c r="E28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>16</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>